<commit_message>
dev-1.0.0 : Update Templete Sales dan Labor
</commit_message>
<xml_diff>
--- a/public/files/Template_Labor_New_2024_New.xlsx
+++ b/public/files/Template_Labor_New_2024_New.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\New Templete 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\Templete yang akan digunakan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E26900-13BF-4DA1-AE3B-FA26B8C2B297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC1D54A-F619-47A1-9AEE-FA31F6DB463D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I44" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1336,7 +1336,9 @@
       <c r="D2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -1350,7 +1352,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="9">
         <f>SUM(E2:J2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="9">
         <f>SUM(K2:P2)</f>
@@ -1358,7 +1360,7 @@
       </c>
       <c r="S2" s="10">
         <f>Q2+R2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
dev-1.0.0 : Update Templete labor
</commit_message>
<xml_diff>
--- a/public/files/Template_Labor_New_2024_New.xlsx
+++ b/public/files/Template_Labor_New_2024_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\Templete yang akan digunakan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC1D54A-F619-47A1-9AEE-FA31F6DB463D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC51D643-C792-4D6C-8493-2724A38D7CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1337,7 +1337,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1352,7 +1352,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="9">
         <f>SUM(E2:J2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" s="9">
         <f>SUM(K2:P2)</f>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="S2" s="10">
         <f>Q2+R2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>